<commit_message>
update: ระบบ PDPA, UI, README, reviewer/admin flow, import ดไซน, bugfix
</commit_message>
<xml_diff>
--- a/CII_SelyAssessment.xlsx
+++ b/CII_SelyAssessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\PDPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A346D4-8978-4064-814C-4BF82760AB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C736F3-4586-4265-8FA1-ED0087496860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{E8DC57B1-CB3D-4366-AC3E-0B3A9EAE7708}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="5" xr2:uid="{E8DC57B1-CB3D-4366-AC3E-0B3A9EAE7708}"/>
   </bookViews>
   <sheets>
     <sheet name="Update Log" sheetId="6" r:id="rId1"/>
@@ -2903,6 +2903,33 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="187" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2929,33 +2956,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7158,20 +7158,20 @@
     </row>
     <row r="5" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="82" t="s">
         <v>382</v>
       </c>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="75"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="84"/>
     </row>
     <row r="7" spans="1:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="87" t="s">
         <v>458</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="80"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="18"/>
       <c r="G7" s="27">
         <f>AVERAGE(G10:G36)</f>
@@ -7184,19 +7184,19 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="85" t="s">
         <v>454</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="88" t="s">
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="79" t="s">
         <v>373</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="86" t="s">
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="77" t="s">
         <v>392</v>
       </c>
     </row>
@@ -7226,7 +7226,7 @@
       <c r="I9" s="29" t="s">
         <v>381</v>
       </c>
-      <c r="J9" s="87"/>
+      <c r="J9" s="78"/>
     </row>
     <row r="10" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.35">
       <c r="A10" s="30">
@@ -7247,14 +7247,14 @@
       <c r="F10" s="23">
         <v>1</v>
       </c>
-      <c r="G10" s="83">
+      <c r="G10" s="73">
         <f>AVERAGE(F10:F14)</f>
         <v>2</v>
       </c>
       <c r="H10" s="23">
         <v>3</v>
       </c>
-      <c r="I10" s="83">
+      <c r="I10" s="73">
         <f>AVERAGE(H10:H14)</f>
         <v>3</v>
       </c>
@@ -7273,11 +7273,11 @@
       <c r="F11" s="24">
         <v>1</v>
       </c>
-      <c r="G11" s="84"/>
+      <c r="G11" s="75"/>
       <c r="H11" s="24">
         <v>3</v>
       </c>
-      <c r="I11" s="84"/>
+      <c r="I11" s="75"/>
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" ht="144.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7293,11 +7293,11 @@
       <c r="F12" s="24">
         <v>2</v>
       </c>
-      <c r="G12" s="84"/>
+      <c r="G12" s="75"/>
       <c r="H12" s="24">
         <v>3</v>
       </c>
-      <c r="I12" s="84"/>
+      <c r="I12" s="75"/>
       <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -7313,11 +7313,11 @@
       <c r="F13" s="24">
         <v>3</v>
       </c>
-      <c r="G13" s="84"/>
+      <c r="G13" s="75"/>
       <c r="H13" s="24">
         <v>3</v>
       </c>
-      <c r="I13" s="84"/>
+      <c r="I13" s="75"/>
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -7333,11 +7333,11 @@
       <c r="F14" s="25">
         <v>3</v>
       </c>
-      <c r="G14" s="85"/>
+      <c r="G14" s="74"/>
       <c r="H14" s="25">
         <v>3</v>
       </c>
-      <c r="I14" s="85"/>
+      <c r="I14" s="74"/>
       <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10" ht="81.599999999999994" x14ac:dyDescent="0.35">
@@ -7359,14 +7359,14 @@
       <c r="F15" s="23">
         <v>1</v>
       </c>
-      <c r="G15" s="83">
+      <c r="G15" s="73">
         <f>AVERAGE(F15:F19)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="H15" s="23">
         <v>3</v>
       </c>
-      <c r="I15" s="83">
+      <c r="I15" s="73">
         <f>AVERAGE(H15:H19)</f>
         <v>3</v>
       </c>
@@ -7385,11 +7385,11 @@
       <c r="F16" s="24">
         <v>2</v>
       </c>
-      <c r="G16" s="84"/>
+      <c r="G16" s="75"/>
       <c r="H16" s="24">
         <v>3</v>
       </c>
-      <c r="I16" s="84"/>
+      <c r="I16" s="75"/>
       <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -7405,11 +7405,11 @@
       <c r="F17" s="24">
         <v>2</v>
       </c>
-      <c r="G17" s="84"/>
+      <c r="G17" s="75"/>
       <c r="H17" s="24">
         <v>3</v>
       </c>
-      <c r="I17" s="84"/>
+      <c r="I17" s="75"/>
       <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" ht="81.599999999999994" x14ac:dyDescent="0.35">
@@ -7425,11 +7425,11 @@
       <c r="F18" s="24">
         <v>3</v>
       </c>
-      <c r="G18" s="84"/>
+      <c r="G18" s="75"/>
       <c r="H18" s="24">
         <v>3</v>
       </c>
-      <c r="I18" s="84"/>
+      <c r="I18" s="75"/>
       <c r="J18" s="16"/>
     </row>
     <row r="19" spans="1:10" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -7445,21 +7445,21 @@
       <c r="F19" s="25">
         <v>3</v>
       </c>
-      <c r="G19" s="85"/>
+      <c r="G19" s="74"/>
       <c r="H19" s="25">
         <v>3</v>
       </c>
-      <c r="I19" s="85"/>
+      <c r="I19" s="74"/>
       <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.35">
-      <c r="A20" s="82">
-        <v>3</v>
-      </c>
-      <c r="B20" s="81" t="s">
+      <c r="A20" s="76">
+        <v>3</v>
+      </c>
+      <c r="B20" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="82" t="s">
+      <c r="C20" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="8">
@@ -7471,23 +7471,23 @@
       <c r="F20" s="23">
         <v>3</v>
       </c>
-      <c r="G20" s="83">
+      <c r="G20" s="73">
         <f>AVERAGE(F20:F22)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="H20" s="23">
         <v>3</v>
       </c>
-      <c r="I20" s="83">
+      <c r="I20" s="73">
         <f>AVERAGE(H20:H22)</f>
         <v>3</v>
       </c>
       <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:10" ht="61.2" x14ac:dyDescent="0.35">
-      <c r="A21" s="82"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="82"/>
+      <c r="A21" s="76"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="8">
         <v>2</v>
       </c>
@@ -7497,17 +7497,17 @@
       <c r="F21" s="24">
         <v>3</v>
       </c>
-      <c r="G21" s="84"/>
+      <c r="G21" s="75"/>
       <c r="H21" s="24">
         <v>3</v>
       </c>
-      <c r="I21" s="84"/>
+      <c r="I21" s="75"/>
       <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="82"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="82"/>
+      <c r="A22" s="76"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="8">
         <v>3</v>
       </c>
@@ -7517,11 +7517,11 @@
       <c r="F22" s="25">
         <v>1</v>
       </c>
-      <c r="G22" s="85"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="25">
         <v>3</v>
       </c>
-      <c r="I22" s="85"/>
+      <c r="I22" s="74"/>
       <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -7639,14 +7639,14 @@
       <c r="F26" s="23">
         <v>3</v>
       </c>
-      <c r="G26" s="83">
+      <c r="G26" s="73">
         <f>AVERAGE(F26:F27)</f>
         <v>3</v>
       </c>
       <c r="H26" s="23">
         <v>3</v>
       </c>
-      <c r="I26" s="83">
+      <c r="I26" s="73">
         <f>AVERAGE(H26:H27)</f>
         <v>3</v>
       </c>
@@ -7665,11 +7665,11 @@
       <c r="F27" s="25">
         <v>3</v>
       </c>
-      <c r="G27" s="85"/>
+      <c r="G27" s="74"/>
       <c r="H27" s="25">
         <v>3</v>
       </c>
-      <c r="I27" s="85"/>
+      <c r="I27" s="74"/>
       <c r="J27" s="16"/>
     </row>
     <row r="28" spans="1:10" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -7787,14 +7787,14 @@
       <c r="F31" s="26">
         <v>3</v>
       </c>
-      <c r="G31" s="83">
+      <c r="G31" s="73">
         <f>AVERAGE(F31:F32)</f>
         <v>3</v>
       </c>
       <c r="H31" s="26">
         <v>3</v>
       </c>
-      <c r="I31" s="83">
+      <c r="I31" s="73">
         <f>AVERAGE(H31:H32)</f>
         <v>3</v>
       </c>
@@ -7813,11 +7813,11 @@
       <c r="F32" s="26">
         <v>3</v>
       </c>
-      <c r="G32" s="85"/>
+      <c r="G32" s="74"/>
       <c r="H32" s="26">
         <v>3</v>
       </c>
-      <c r="I32" s="85"/>
+      <c r="I32" s="74"/>
       <c r="J32" s="16"/>
     </row>
     <row r="33" spans="1:10" ht="354.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7839,14 +7839,14 @@
       <c r="F33" s="23">
         <v>3</v>
       </c>
-      <c r="G33" s="83">
+      <c r="G33" s="73">
         <f>AVERAGE(F33:F36)</f>
         <v>3</v>
       </c>
       <c r="H33" s="23">
         <v>3</v>
       </c>
-      <c r="I33" s="83">
+      <c r="I33" s="73">
         <f>AVERAGE(H33:H36)</f>
         <v>3</v>
       </c>
@@ -7865,11 +7865,11 @@
       <c r="F34" s="24">
         <v>3</v>
       </c>
-      <c r="G34" s="84"/>
+      <c r="G34" s="75"/>
       <c r="H34" s="24">
         <v>3</v>
       </c>
-      <c r="I34" s="84"/>
+      <c r="I34" s="75"/>
       <c r="J34" s="16"/>
     </row>
     <row r="35" spans="1:10" ht="61.2" x14ac:dyDescent="0.35">
@@ -7885,11 +7885,11 @@
       <c r="F35" s="24">
         <v>3</v>
       </c>
-      <c r="G35" s="84"/>
+      <c r="G35" s="75"/>
       <c r="H35" s="24">
         <v>3</v>
       </c>
-      <c r="I35" s="84"/>
+      <c r="I35" s="75"/>
       <c r="J35" s="16"/>
     </row>
     <row r="36" spans="1:10" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -7905,11 +7905,11 @@
       <c r="F36" s="25">
         <v>3</v>
       </c>
-      <c r="G36" s="85"/>
+      <c r="G36" s="74"/>
       <c r="H36" s="25">
         <v>3</v>
       </c>
-      <c r="I36" s="85"/>
+      <c r="I36" s="74"/>
       <c r="J36" s="16"/>
     </row>
     <row r="38" spans="1:10" ht="24.6" x14ac:dyDescent="0.35">
@@ -7923,6 +7923,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="G10:G14"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="F8:I8"/>
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="G31:G32"/>
     <mergeCell ref="G33:G36"/>
@@ -7932,17 +7943,6 @@
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="I31:I32"/>
     <mergeCell ref="I33:I36"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="G10:G14"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G19">
     <cfRule type="cellIs" dxfId="509" priority="58" operator="between">
@@ -8287,12 +8287,12 @@
     </row>
     <row r="5" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="82" t="s">
         <v>382</v>
       </c>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="75"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="84"/>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -8321,13 +8321,13 @@
       <c r="C8" s="92"/>
       <c r="D8" s="92"/>
       <c r="E8" s="93"/>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="79" t="s">
         <v>373</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="86" t="s">
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="77" t="s">
         <v>392</v>
       </c>
     </row>
@@ -8357,7 +8357,7 @@
       <c r="I9" s="29" t="s">
         <v>381</v>
       </c>
-      <c r="J9" s="87"/>
+      <c r="J9" s="78"/>
     </row>
     <row r="10" spans="1:10" ht="123" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="8">
@@ -8906,12 +8906,12 @@
     </row>
     <row r="5" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="82" t="s">
         <v>382</v>
       </c>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="75"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
     </row>
     <row r="7" spans="1:11" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="94" t="s">
@@ -8940,13 +8940,13 @@
       <c r="D8" s="92"/>
       <c r="E8" s="92"/>
       <c r="F8" s="93"/>
-      <c r="G8" s="88" t="s">
+      <c r="G8" s="79" t="s">
         <v>373</v>
       </c>
-      <c r="H8" s="89"/>
-      <c r="I8" s="89"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="86" t="s">
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="77" t="s">
         <v>392</v>
       </c>
     </row>
@@ -8979,7 +8979,7 @@
       <c r="J9" s="29" t="s">
         <v>381</v>
       </c>
-      <c r="K9" s="87"/>
+      <c r="K9" s="78"/>
     </row>
     <row r="10" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="8">
@@ -9038,14 +9038,14 @@
       <c r="G11" s="23">
         <v>3</v>
       </c>
-      <c r="H11" s="83">
+      <c r="H11" s="73">
         <f>AVERAGE(G11:G13)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I11" s="23">
         <v>3</v>
       </c>
-      <c r="J11" s="83">
+      <c r="J11" s="73">
         <f>AVERAGE(I11:I13)</f>
         <v>3</v>
       </c>
@@ -9067,11 +9067,11 @@
       <c r="G12" s="24">
         <v>3</v>
       </c>
-      <c r="H12" s="84"/>
+      <c r="H12" s="75"/>
       <c r="I12" s="24">
         <v>3</v>
       </c>
-      <c r="J12" s="84"/>
+      <c r="J12" s="75"/>
       <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -9090,11 +9090,11 @@
       <c r="G13" s="25">
         <v>1</v>
       </c>
-      <c r="H13" s="85"/>
+      <c r="H13" s="74"/>
       <c r="I13" s="25">
         <v>3</v>
       </c>
-      <c r="J13" s="85"/>
+      <c r="J13" s="74"/>
       <c r="K13" s="31"/>
     </row>
     <row r="14" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -9119,14 +9119,14 @@
       <c r="G14" s="23">
         <v>3</v>
       </c>
-      <c r="H14" s="83">
+      <c r="H14" s="73">
         <f>AVERAGE(G14:G18)</f>
         <v>2.6</v>
       </c>
       <c r="I14" s="23">
         <v>3</v>
       </c>
-      <c r="J14" s="83">
+      <c r="J14" s="73">
         <f>AVERAGE(I14:I18)</f>
         <v>3</v>
       </c>
@@ -9146,11 +9146,11 @@
       <c r="G15" s="24">
         <v>2</v>
       </c>
-      <c r="H15" s="84"/>
+      <c r="H15" s="75"/>
       <c r="I15" s="24">
         <v>3</v>
       </c>
-      <c r="J15" s="84"/>
+      <c r="J15" s="75"/>
       <c r="K15" s="31"/>
     </row>
     <row r="16" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -9167,11 +9167,11 @@
       <c r="G16" s="24">
         <v>2</v>
       </c>
-      <c r="H16" s="84"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="24">
         <v>3</v>
       </c>
-      <c r="J16" s="84"/>
+      <c r="J16" s="75"/>
       <c r="K16" s="31"/>
     </row>
     <row r="17" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -9188,11 +9188,11 @@
       <c r="G17" s="24">
         <v>3</v>
       </c>
-      <c r="H17" s="84"/>
+      <c r="H17" s="75"/>
       <c r="I17" s="24">
         <v>3</v>
       </c>
-      <c r="J17" s="84"/>
+      <c r="J17" s="75"/>
       <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -9209,11 +9209,11 @@
       <c r="G18" s="25">
         <v>3</v>
       </c>
-      <c r="H18" s="85"/>
+      <c r="H18" s="74"/>
       <c r="I18" s="25">
         <v>3</v>
       </c>
-      <c r="J18" s="85"/>
+      <c r="J18" s="74"/>
       <c r="K18" s="31"/>
     </row>
     <row r="19" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -9238,14 +9238,14 @@
       <c r="G19" s="23">
         <v>3</v>
       </c>
-      <c r="H19" s="83">
+      <c r="H19" s="73">
         <f>AVERAGE(G19:G22)</f>
         <v>3</v>
       </c>
       <c r="I19" s="23">
         <v>3</v>
       </c>
-      <c r="J19" s="83">
+      <c r="J19" s="73">
         <f>AVERAGE(I19:I22)</f>
         <v>3</v>
       </c>
@@ -9267,11 +9267,11 @@
       <c r="G20" s="24">
         <v>3</v>
       </c>
-      <c r="H20" s="84"/>
+      <c r="H20" s="75"/>
       <c r="I20" s="24">
         <v>3</v>
       </c>
-      <c r="J20" s="84"/>
+      <c r="J20" s="75"/>
       <c r="K20" s="31"/>
     </row>
     <row r="21" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -9289,11 +9289,11 @@
       <c r="G21" s="24">
         <v>3</v>
       </c>
-      <c r="H21" s="84"/>
+      <c r="H21" s="75"/>
       <c r="I21" s="24">
         <v>3</v>
       </c>
-      <c r="J21" s="84"/>
+      <c r="J21" s="75"/>
       <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -9312,11 +9312,11 @@
       <c r="G22" s="25">
         <v>3</v>
       </c>
-      <c r="H22" s="85"/>
+      <c r="H22" s="74"/>
       <c r="I22" s="25">
         <v>3</v>
       </c>
-      <c r="J22" s="85"/>
+      <c r="J22" s="74"/>
       <c r="K22" s="31"/>
     </row>
     <row r="23" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -9376,14 +9376,14 @@
       <c r="G24" s="26">
         <v>3</v>
       </c>
-      <c r="H24" s="83">
+      <c r="H24" s="73">
         <f>AVERAGE(G24:G25)</f>
         <v>3</v>
       </c>
       <c r="I24" s="26">
         <v>3</v>
       </c>
-      <c r="J24" s="83">
+      <c r="J24" s="73">
         <f>AVERAGE(I24:I25)</f>
         <v>3</v>
       </c>
@@ -9403,11 +9403,11 @@
       <c r="G25" s="26">
         <v>3</v>
       </c>
-      <c r="H25" s="85"/>
+      <c r="H25" s="74"/>
       <c r="I25" s="26">
         <v>3</v>
       </c>
-      <c r="J25" s="85"/>
+      <c r="J25" s="74"/>
       <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" ht="184.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -9432,14 +9432,14 @@
       <c r="G26" s="26">
         <v>3</v>
       </c>
-      <c r="H26" s="83">
+      <c r="H26" s="73">
         <f>AVERAGE(G26:G27)</f>
         <v>3</v>
       </c>
       <c r="I26" s="26">
         <v>3</v>
       </c>
-      <c r="J26" s="83">
+      <c r="J26" s="73">
         <f>AVERAGE(I26:I27)</f>
         <v>3</v>
       </c>
@@ -9459,11 +9459,11 @@
       <c r="G27" s="26">
         <v>3</v>
       </c>
-      <c r="H27" s="85"/>
+      <c r="H27" s="74"/>
       <c r="I27" s="26">
         <v>3</v>
       </c>
-      <c r="J27" s="85"/>
+      <c r="J27" s="74"/>
       <c r="K27" s="31"/>
     </row>
     <row r="28" spans="1:11" ht="102" x14ac:dyDescent="0.35">
@@ -9488,14 +9488,14 @@
       <c r="G28" s="23">
         <v>3</v>
       </c>
-      <c r="H28" s="83">
+      <c r="H28" s="73">
         <f>AVERAGE(G28:G30)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I28" s="23">
         <v>3</v>
       </c>
-      <c r="J28" s="83">
+      <c r="J28" s="73">
         <f>AVERAGE(I28:I30)</f>
         <v>3</v>
       </c>
@@ -9515,11 +9515,11 @@
       <c r="G29" s="24">
         <v>3</v>
       </c>
-      <c r="H29" s="84"/>
+      <c r="H29" s="75"/>
       <c r="I29" s="24">
         <v>3</v>
       </c>
-      <c r="J29" s="84"/>
+      <c r="J29" s="75"/>
       <c r="K29" s="31"/>
     </row>
     <row r="30" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -9536,11 +9536,11 @@
       <c r="G30" s="25">
         <v>1</v>
       </c>
-      <c r="H30" s="85"/>
+      <c r="H30" s="74"/>
       <c r="I30" s="25">
         <v>3</v>
       </c>
-      <c r="J30" s="85"/>
+      <c r="J30" s="74"/>
       <c r="K30" s="31"/>
     </row>
     <row r="31" spans="1:11" ht="102.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -9565,14 +9565,14 @@
       <c r="G31" s="26">
         <v>3</v>
       </c>
-      <c r="H31" s="83">
+      <c r="H31" s="73">
         <f>AVERAGE(G31:G32)</f>
         <v>3</v>
       </c>
       <c r="I31" s="26">
         <v>3</v>
       </c>
-      <c r="J31" s="83">
+      <c r="J31" s="73">
         <f>AVERAGE(I31:I32)</f>
         <v>3</v>
       </c>
@@ -9592,11 +9592,11 @@
       <c r="G32" s="26">
         <v>3</v>
       </c>
-      <c r="H32" s="85"/>
+      <c r="H32" s="74"/>
       <c r="I32" s="26">
         <v>3</v>
       </c>
-      <c r="J32" s="85"/>
+      <c r="J32" s="74"/>
       <c r="K32" s="31"/>
     </row>
     <row r="33" spans="1:11" ht="118.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -9691,14 +9691,14 @@
       <c r="G35" s="26">
         <v>3</v>
       </c>
-      <c r="H35" s="83">
+      <c r="H35" s="73">
         <f>AVERAGE(G35:G36)</f>
         <v>3</v>
       </c>
       <c r="I35" s="26">
         <v>3</v>
       </c>
-      <c r="J35" s="83">
+      <c r="J35" s="73">
         <f>AVERAGE(I35:I36)</f>
         <v>3</v>
       </c>
@@ -9718,11 +9718,11 @@
       <c r="G36" s="26">
         <v>3</v>
       </c>
-      <c r="H36" s="85"/>
+      <c r="H36" s="74"/>
       <c r="I36" s="26">
         <v>3</v>
       </c>
-      <c r="J36" s="85"/>
+      <c r="J36" s="74"/>
       <c r="K36" s="31"/>
     </row>
     <row r="37" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -9760,7 +9760,7 @@
       </c>
       <c r="K37" s="31"/>
     </row>
-    <row r="38" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" ht="102.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="8">
         <v>39</v>
       </c>
@@ -9817,14 +9817,14 @@
       <c r="G39" s="26">
         <v>3</v>
       </c>
-      <c r="H39" s="83">
+      <c r="H39" s="73">
         <f>AVERAGE(G39:G40)</f>
         <v>3</v>
       </c>
       <c r="I39" s="26">
         <v>3</v>
       </c>
-      <c r="J39" s="83">
+      <c r="J39" s="73">
         <f>AVERAGE(I39:I40)</f>
         <v>3</v>
       </c>
@@ -9844,11 +9844,11 @@
       <c r="G40" s="26">
         <v>3</v>
       </c>
-      <c r="H40" s="85"/>
+      <c r="H40" s="74"/>
       <c r="I40" s="26">
         <v>3</v>
       </c>
-      <c r="J40" s="85"/>
+      <c r="J40" s="74"/>
       <c r="K40" s="31"/>
     </row>
     <row r="41" spans="1:11" ht="102" x14ac:dyDescent="0.35">
@@ -9873,14 +9873,14 @@
       <c r="G41" s="23">
         <v>3</v>
       </c>
-      <c r="H41" s="83">
+      <c r="H41" s="73">
         <f>AVERAGE(G41:G43)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I41" s="23">
         <v>3</v>
       </c>
-      <c r="J41" s="83">
+      <c r="J41" s="73">
         <f>AVERAGE(I41:I43)</f>
         <v>3</v>
       </c>
@@ -9900,11 +9900,11 @@
       <c r="G42" s="24">
         <v>3</v>
       </c>
-      <c r="H42" s="84"/>
+      <c r="H42" s="75"/>
       <c r="I42" s="24">
         <v>3</v>
       </c>
-      <c r="J42" s="84"/>
+      <c r="J42" s="75"/>
       <c r="K42" s="31"/>
     </row>
     <row r="43" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -9921,11 +9921,11 @@
       <c r="G43" s="25">
         <v>1</v>
       </c>
-      <c r="H43" s="85"/>
+      <c r="H43" s="74"/>
       <c r="I43" s="25">
         <v>3</v>
       </c>
-      <c r="J43" s="85"/>
+      <c r="J43" s="74"/>
       <c r="K43" s="31"/>
     </row>
     <row r="44" spans="1:11" ht="102" x14ac:dyDescent="0.35">
@@ -9950,14 +9950,14 @@
       <c r="G44" s="23">
         <v>3</v>
       </c>
-      <c r="H44" s="83">
+      <c r="H44" s="73">
         <f>AVERAGE(G44:G46)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I44" s="23">
         <v>3</v>
       </c>
-      <c r="J44" s="83">
+      <c r="J44" s="73">
         <f>AVERAGE(I44:I46)</f>
         <v>3</v>
       </c>
@@ -9977,11 +9977,11 @@
       <c r="G45" s="24">
         <v>3</v>
       </c>
-      <c r="H45" s="84"/>
+      <c r="H45" s="75"/>
       <c r="I45" s="24">
         <v>3</v>
       </c>
-      <c r="J45" s="84"/>
+      <c r="J45" s="75"/>
       <c r="K45" s="31"/>
     </row>
     <row r="46" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -9998,11 +9998,11 @@
       <c r="G46" s="25">
         <v>1</v>
       </c>
-      <c r="H46" s="85"/>
+      <c r="H46" s="74"/>
       <c r="I46" s="25">
         <v>3</v>
       </c>
-      <c r="J46" s="85"/>
+      <c r="J46" s="74"/>
       <c r="K46" s="31"/>
     </row>
     <row r="47" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -10027,14 +10027,14 @@
       <c r="G47" s="26">
         <v>3</v>
       </c>
-      <c r="H47" s="83">
+      <c r="H47" s="73">
         <f>AVERAGE(G47:G48)</f>
         <v>3</v>
       </c>
       <c r="I47" s="26">
         <v>3</v>
       </c>
-      <c r="J47" s="83">
+      <c r="J47" s="73">
         <f>AVERAGE(I47:I48)</f>
         <v>3</v>
       </c>
@@ -10054,11 +10054,11 @@
       <c r="G48" s="26">
         <v>3</v>
       </c>
-      <c r="H48" s="85"/>
+      <c r="H48" s="74"/>
       <c r="I48" s="26">
         <v>3</v>
       </c>
-      <c r="J48" s="85"/>
+      <c r="J48" s="74"/>
       <c r="K48" s="31"/>
     </row>
     <row r="49" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -10083,14 +10083,14 @@
       <c r="G49" s="23">
         <v>1</v>
       </c>
-      <c r="H49" s="83">
+      <c r="H49" s="73">
         <f>AVERAGE(G49:G53)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I49" s="23">
         <v>3</v>
       </c>
-      <c r="J49" s="83">
+      <c r="J49" s="73">
         <f>AVERAGE(I49:I53)</f>
         <v>3</v>
       </c>
@@ -10110,11 +10110,11 @@
       <c r="G50" s="24">
         <v>2</v>
       </c>
-      <c r="H50" s="84"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="24">
         <v>3</v>
       </c>
-      <c r="J50" s="84"/>
+      <c r="J50" s="75"/>
       <c r="K50" s="31"/>
     </row>
     <row r="51" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -10130,11 +10130,11 @@
       <c r="G51" s="24">
         <v>2</v>
       </c>
-      <c r="H51" s="84"/>
+      <c r="H51" s="75"/>
       <c r="I51" s="24">
         <v>3</v>
       </c>
-      <c r="J51" s="84"/>
+      <c r="J51" s="75"/>
       <c r="K51" s="31"/>
     </row>
     <row r="52" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -10150,11 +10150,11 @@
       <c r="G52" s="24">
         <v>3</v>
       </c>
-      <c r="H52" s="84"/>
+      <c r="H52" s="75"/>
       <c r="I52" s="24">
         <v>3</v>
       </c>
-      <c r="J52" s="84"/>
+      <c r="J52" s="75"/>
       <c r="K52" s="31"/>
     </row>
     <row r="53" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -10171,11 +10171,11 @@
       <c r="G53" s="25">
         <v>3</v>
       </c>
-      <c r="H53" s="85"/>
+      <c r="H53" s="74"/>
       <c r="I53" s="25">
         <v>3</v>
       </c>
-      <c r="J53" s="85"/>
+      <c r="J53" s="74"/>
       <c r="K53" s="31"/>
     </row>
     <row r="54" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -10200,14 +10200,14 @@
       <c r="G54" s="26">
         <v>3</v>
       </c>
-      <c r="H54" s="83">
+      <c r="H54" s="73">
         <f>AVERAGE(G54:G55)</f>
         <v>3</v>
       </c>
       <c r="I54" s="26">
         <v>3</v>
       </c>
-      <c r="J54" s="83">
+      <c r="J54" s="73">
         <f>AVERAGE(I54:I55)</f>
         <v>3</v>
       </c>
@@ -10227,11 +10227,11 @@
       <c r="G55" s="26">
         <v>3</v>
       </c>
-      <c r="H55" s="85"/>
+      <c r="H55" s="74"/>
       <c r="I55" s="26">
         <v>3</v>
       </c>
-      <c r="J55" s="85"/>
+      <c r="J55" s="74"/>
       <c r="K55" s="31"/>
     </row>
     <row r="56" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -10256,14 +10256,14 @@
       <c r="G56" s="23">
         <v>3</v>
       </c>
-      <c r="H56" s="83">
+      <c r="H56" s="73">
         <f>AVERAGE(G56:G58)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I56" s="23">
         <v>3</v>
       </c>
-      <c r="J56" s="83">
+      <c r="J56" s="73">
         <f>AVERAGE(I56:I58)</f>
         <v>3</v>
       </c>
@@ -10285,11 +10285,11 @@
       <c r="G57" s="24">
         <v>3</v>
       </c>
-      <c r="H57" s="84"/>
+      <c r="H57" s="75"/>
       <c r="I57" s="24">
         <v>3</v>
       </c>
-      <c r="J57" s="84"/>
+      <c r="J57" s="75"/>
       <c r="K57" s="31"/>
     </row>
     <row r="58" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -10306,11 +10306,11 @@
       <c r="G58" s="25">
         <v>1</v>
       </c>
-      <c r="H58" s="85"/>
+      <c r="H58" s="74"/>
       <c r="I58" s="25">
         <v>3</v>
       </c>
-      <c r="J58" s="85"/>
+      <c r="J58" s="74"/>
       <c r="K58" s="31"/>
     </row>
     <row r="59" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -10440,14 +10440,14 @@
       <c r="G62" s="26">
         <v>3</v>
       </c>
-      <c r="H62" s="83">
+      <c r="H62" s="73">
         <f>AVERAGE(G62:G63)</f>
         <v>3</v>
       </c>
       <c r="I62" s="26">
         <v>3</v>
       </c>
-      <c r="J62" s="83">
+      <c r="J62" s="73">
         <f>AVERAGE(I62:I63)</f>
         <v>3</v>
       </c>
@@ -10467,11 +10467,11 @@
       <c r="G63" s="26">
         <v>3</v>
       </c>
-      <c r="H63" s="85"/>
+      <c r="H63" s="74"/>
       <c r="I63" s="26">
         <v>3</v>
       </c>
-      <c r="J63" s="85"/>
+      <c r="J63" s="74"/>
       <c r="K63" s="31"/>
     </row>
     <row r="64" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -10496,14 +10496,14 @@
       <c r="G64" s="23">
         <v>1</v>
       </c>
-      <c r="H64" s="83">
+      <c r="H64" s="73">
         <f>AVERAGE(G64:G68)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I64" s="23">
         <v>3</v>
       </c>
-      <c r="J64" s="83">
+      <c r="J64" s="73">
         <f>AVERAGE(I64:I68)</f>
         <v>3</v>
       </c>
@@ -10523,11 +10523,11 @@
       <c r="G65" s="24">
         <v>2</v>
       </c>
-      <c r="H65" s="84"/>
+      <c r="H65" s="75"/>
       <c r="I65" s="24">
         <v>3</v>
       </c>
-      <c r="J65" s="84"/>
+      <c r="J65" s="75"/>
       <c r="K65" s="31"/>
     </row>
     <row r="66" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -10543,11 +10543,11 @@
       <c r="G66" s="24">
         <v>2</v>
       </c>
-      <c r="H66" s="84"/>
+      <c r="H66" s="75"/>
       <c r="I66" s="24">
         <v>3</v>
       </c>
-      <c r="J66" s="84"/>
+      <c r="J66" s="75"/>
       <c r="K66" s="31"/>
     </row>
     <row r="67" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -10563,11 +10563,11 @@
       <c r="G67" s="24">
         <v>3</v>
       </c>
-      <c r="H67" s="84"/>
+      <c r="H67" s="75"/>
       <c r="I67" s="24">
         <v>3</v>
       </c>
-      <c r="J67" s="84"/>
+      <c r="J67" s="75"/>
       <c r="K67" s="31"/>
     </row>
     <row r="68" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -10584,11 +10584,11 @@
       <c r="G68" s="25">
         <v>3</v>
       </c>
-      <c r="H68" s="85"/>
+      <c r="H68" s="74"/>
       <c r="I68" s="25">
         <v>3</v>
       </c>
-      <c r="J68" s="85"/>
+      <c r="J68" s="74"/>
       <c r="K68" s="31"/>
     </row>
     <row r="69" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -10718,14 +10718,14 @@
       <c r="G72" s="26">
         <v>3</v>
       </c>
-      <c r="H72" s="83">
+      <c r="H72" s="73">
         <f>AVERAGE(G72:G73)</f>
         <v>3</v>
       </c>
       <c r="I72" s="26">
         <v>3</v>
       </c>
-      <c r="J72" s="83">
+      <c r="J72" s="73">
         <f>AVERAGE(I72:I73)</f>
         <v>3</v>
       </c>
@@ -10745,11 +10745,11 @@
       <c r="G73" s="26">
         <v>3</v>
       </c>
-      <c r="H73" s="85"/>
+      <c r="H73" s="74"/>
       <c r="I73" s="26">
         <v>3</v>
       </c>
-      <c r="J73" s="85"/>
+      <c r="J73" s="74"/>
       <c r="K73" s="31"/>
     </row>
     <row r="74" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -10809,14 +10809,14 @@
       <c r="G75" s="23">
         <v>3</v>
       </c>
-      <c r="H75" s="83">
+      <c r="H75" s="73">
         <f>AVERAGE(G75:G77)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I75" s="23">
         <v>3</v>
       </c>
-      <c r="J75" s="83">
+      <c r="J75" s="73">
         <f>AVERAGE(I75:I77)</f>
         <v>3</v>
       </c>
@@ -10836,11 +10836,11 @@
       <c r="G76" s="24">
         <v>3</v>
       </c>
-      <c r="H76" s="84"/>
+      <c r="H76" s="75"/>
       <c r="I76" s="24">
         <v>3</v>
       </c>
-      <c r="J76" s="84"/>
+      <c r="J76" s="75"/>
       <c r="K76" s="31"/>
     </row>
     <row r="77" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -10857,11 +10857,11 @@
       <c r="G77" s="25">
         <v>1</v>
       </c>
-      <c r="H77" s="85"/>
+      <c r="H77" s="74"/>
       <c r="I77" s="25">
         <v>3</v>
       </c>
-      <c r="J77" s="85"/>
+      <c r="J77" s="74"/>
       <c r="K77" s="31"/>
     </row>
     <row r="78" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -10921,14 +10921,14 @@
       <c r="G79" s="26">
         <v>3</v>
       </c>
-      <c r="H79" s="83">
+      <c r="H79" s="73">
         <f>AVERAGE(G79:G80)</f>
         <v>3</v>
       </c>
       <c r="I79" s="26">
         <v>3</v>
       </c>
-      <c r="J79" s="83">
+      <c r="J79" s="73">
         <f>AVERAGE(I79:I80)</f>
         <v>3</v>
       </c>
@@ -10948,11 +10948,11 @@
       <c r="G80" s="26">
         <v>3</v>
       </c>
-      <c r="H80" s="85"/>
+      <c r="H80" s="74"/>
       <c r="I80" s="26">
         <v>3</v>
       </c>
-      <c r="J80" s="85"/>
+      <c r="J80" s="74"/>
       <c r="K80" s="31"/>
     </row>
     <row r="81" spans="1:11" ht="102.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -10977,14 +10977,14 @@
       <c r="G81" s="26">
         <v>3</v>
       </c>
-      <c r="H81" s="83">
+      <c r="H81" s="73">
         <f>AVERAGE(G81:G82)</f>
         <v>3</v>
       </c>
       <c r="I81" s="26">
         <v>3</v>
       </c>
-      <c r="J81" s="83">
+      <c r="J81" s="73">
         <f>AVERAGE(I81:I82)</f>
         <v>3</v>
       </c>
@@ -11004,11 +11004,11 @@
       <c r="G82" s="26">
         <v>3</v>
       </c>
-      <c r="H82" s="85"/>
+      <c r="H82" s="74"/>
       <c r="I82" s="26">
         <v>3</v>
       </c>
-      <c r="J82" s="85"/>
+      <c r="J82" s="74"/>
       <c r="K82" s="31"/>
     </row>
     <row r="83" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -11033,14 +11033,14 @@
       <c r="G83" s="26">
         <v>3</v>
       </c>
-      <c r="H83" s="83">
+      <c r="H83" s="73">
         <f>AVERAGE(G83:G84)</f>
         <v>3</v>
       </c>
       <c r="I83" s="26">
         <v>3</v>
       </c>
-      <c r="J83" s="83">
+      <c r="J83" s="73">
         <f>AVERAGE(I83:I84)</f>
         <v>3</v>
       </c>
@@ -11060,11 +11060,11 @@
       <c r="G84" s="26">
         <v>3</v>
       </c>
-      <c r="H84" s="85"/>
+      <c r="H84" s="74"/>
       <c r="I84" s="26">
         <v>3</v>
       </c>
-      <c r="J84" s="85"/>
+      <c r="J84" s="74"/>
       <c r="K84" s="31"/>
     </row>
     <row r="85" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -11124,14 +11124,14 @@
       <c r="G86" s="26">
         <v>3</v>
       </c>
-      <c r="H86" s="83">
+      <c r="H86" s="73">
         <f>AVERAGE(G86:G87)</f>
         <v>3</v>
       </c>
       <c r="I86" s="26">
         <v>3</v>
       </c>
-      <c r="J86" s="83">
+      <c r="J86" s="73">
         <f>AVERAGE(I86:I87)</f>
         <v>3</v>
       </c>
@@ -11151,11 +11151,11 @@
       <c r="G87" s="26">
         <v>3</v>
       </c>
-      <c r="H87" s="85"/>
+      <c r="H87" s="74"/>
       <c r="I87" s="26">
         <v>3</v>
       </c>
-      <c r="J87" s="85"/>
+      <c r="J87" s="74"/>
       <c r="K87" s="31"/>
     </row>
     <row r="88" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -11180,14 +11180,14 @@
       <c r="G88" s="23">
         <v>3</v>
       </c>
-      <c r="H88" s="83">
+      <c r="H88" s="73">
         <f>AVERAGE(G88:G90)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I88" s="23">
         <v>3</v>
       </c>
-      <c r="J88" s="83">
+      <c r="J88" s="73">
         <f>AVERAGE(I88:I90)</f>
         <v>3</v>
       </c>
@@ -11207,11 +11207,11 @@
       <c r="G89" s="24">
         <v>3</v>
       </c>
-      <c r="H89" s="84"/>
+      <c r="H89" s="75"/>
       <c r="I89" s="24">
         <v>3</v>
       </c>
-      <c r="J89" s="84"/>
+      <c r="J89" s="75"/>
       <c r="K89" s="31"/>
     </row>
     <row r="90" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -11228,11 +11228,11 @@
       <c r="G90" s="25">
         <v>1</v>
       </c>
-      <c r="H90" s="85"/>
+      <c r="H90" s="74"/>
       <c r="I90" s="25">
         <v>3</v>
       </c>
-      <c r="J90" s="85"/>
+      <c r="J90" s="74"/>
       <c r="K90" s="31"/>
     </row>
     <row r="91" spans="1:11" ht="102.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -11257,14 +11257,14 @@
       <c r="G91" s="25">
         <v>1</v>
       </c>
-      <c r="H91" s="83">
+      <c r="H91" s="73">
         <f>AVERAGE(G91:G105)</f>
         <v>1.5333333333333334</v>
       </c>
       <c r="I91" s="26">
         <v>3</v>
       </c>
-      <c r="J91" s="83">
+      <c r="J91" s="73">
         <f>AVERAGE(I91:I105)</f>
         <v>3</v>
       </c>
@@ -11284,11 +11284,11 @@
       <c r="G92" s="25">
         <v>1</v>
       </c>
-      <c r="H92" s="84"/>
+      <c r="H92" s="75"/>
       <c r="I92" s="26">
         <v>3</v>
       </c>
-      <c r="J92" s="84"/>
+      <c r="J92" s="75"/>
       <c r="K92" s="31"/>
     </row>
     <row r="93" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -11304,11 +11304,11 @@
       <c r="G93" s="25">
         <v>1</v>
       </c>
-      <c r="H93" s="84"/>
+      <c r="H93" s="75"/>
       <c r="I93" s="26">
         <v>3</v>
       </c>
-      <c r="J93" s="84"/>
+      <c r="J93" s="75"/>
       <c r="K93" s="31"/>
     </row>
     <row r="94" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -11324,11 +11324,11 @@
       <c r="G94" s="25">
         <v>1</v>
       </c>
-      <c r="H94" s="84"/>
+      <c r="H94" s="75"/>
       <c r="I94" s="26">
         <v>3</v>
       </c>
-      <c r="J94" s="84"/>
+      <c r="J94" s="75"/>
       <c r="K94" s="31"/>
     </row>
     <row r="95" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11344,11 +11344,11 @@
       <c r="G95" s="25">
         <v>2</v>
       </c>
-      <c r="H95" s="84"/>
+      <c r="H95" s="75"/>
       <c r="I95" s="26">
         <v>3</v>
       </c>
-      <c r="J95" s="84"/>
+      <c r="J95" s="75"/>
       <c r="K95" s="31"/>
     </row>
     <row r="96" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11364,11 +11364,11 @@
       <c r="G96" s="25">
         <v>1</v>
       </c>
-      <c r="H96" s="84"/>
+      <c r="H96" s="75"/>
       <c r="I96" s="26">
         <v>3</v>
       </c>
-      <c r="J96" s="84"/>
+      <c r="J96" s="75"/>
       <c r="K96" s="31"/>
     </row>
     <row r="97" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -11384,11 +11384,11 @@
       <c r="G97" s="25">
         <v>1</v>
       </c>
-      <c r="H97" s="84"/>
+      <c r="H97" s="75"/>
       <c r="I97" s="26">
         <v>3</v>
       </c>
-      <c r="J97" s="84"/>
+      <c r="J97" s="75"/>
       <c r="K97" s="31"/>
     </row>
     <row r="98" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -11404,11 +11404,11 @@
       <c r="G98" s="25">
         <v>2</v>
       </c>
-      <c r="H98" s="84"/>
+      <c r="H98" s="75"/>
       <c r="I98" s="26">
         <v>3</v>
       </c>
-      <c r="J98" s="84"/>
+      <c r="J98" s="75"/>
       <c r="K98" s="31"/>
     </row>
     <row r="99" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -11424,11 +11424,11 @@
       <c r="G99" s="25">
         <v>1</v>
       </c>
-      <c r="H99" s="84"/>
+      <c r="H99" s="75"/>
       <c r="I99" s="26">
         <v>3</v>
       </c>
-      <c r="J99" s="84"/>
+      <c r="J99" s="75"/>
       <c r="K99" s="31"/>
     </row>
     <row r="100" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11444,11 +11444,11 @@
       <c r="G100" s="25">
         <v>3</v>
       </c>
-      <c r="H100" s="84"/>
+      <c r="H100" s="75"/>
       <c r="I100" s="26">
         <v>3</v>
       </c>
-      <c r="J100" s="84"/>
+      <c r="J100" s="75"/>
       <c r="K100" s="31"/>
     </row>
     <row r="101" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11464,11 +11464,11 @@
       <c r="G101" s="25">
         <v>1</v>
       </c>
-      <c r="H101" s="84"/>
+      <c r="H101" s="75"/>
       <c r="I101" s="26">
         <v>3</v>
       </c>
-      <c r="J101" s="84"/>
+      <c r="J101" s="75"/>
       <c r="K101" s="31"/>
     </row>
     <row r="102" spans="1:11" ht="102.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -11484,11 +11484,11 @@
       <c r="G102" s="25">
         <v>3</v>
       </c>
-      <c r="H102" s="84"/>
+      <c r="H102" s="75"/>
       <c r="I102" s="26">
         <v>3</v>
       </c>
-      <c r="J102" s="84"/>
+      <c r="J102" s="75"/>
       <c r="K102" s="31"/>
     </row>
     <row r="103" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -11504,11 +11504,11 @@
       <c r="G103" s="25">
         <v>3</v>
       </c>
-      <c r="H103" s="84"/>
+      <c r="H103" s="75"/>
       <c r="I103" s="26">
         <v>3</v>
       </c>
-      <c r="J103" s="84"/>
+      <c r="J103" s="75"/>
       <c r="K103" s="31"/>
     </row>
     <row r="104" spans="1:11" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -11524,11 +11524,11 @@
       <c r="G104" s="25">
         <v>1</v>
       </c>
-      <c r="H104" s="84"/>
+      <c r="H104" s="75"/>
       <c r="I104" s="26">
         <v>3</v>
       </c>
-      <c r="J104" s="84"/>
+      <c r="J104" s="75"/>
       <c r="K104" s="31"/>
     </row>
     <row r="105" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -11545,11 +11545,11 @@
       <c r="G105" s="25">
         <v>1</v>
       </c>
-      <c r="H105" s="85"/>
+      <c r="H105" s="74"/>
       <c r="I105" s="26">
         <v>3</v>
       </c>
-      <c r="J105" s="85"/>
+      <c r="J105" s="74"/>
       <c r="K105" s="31"/>
     </row>
     <row r="106" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11574,14 +11574,14 @@
       <c r="G106" s="26">
         <v>3</v>
       </c>
-      <c r="H106" s="83">
+      <c r="H106" s="73">
         <f>AVERAGE(G106:G107)</f>
         <v>3</v>
       </c>
       <c r="I106" s="26">
         <v>3</v>
       </c>
-      <c r="J106" s="83">
+      <c r="J106" s="73">
         <f>AVERAGE(I106:I107)</f>
         <v>3</v>
       </c>
@@ -11601,11 +11601,11 @@
       <c r="G107" s="26">
         <v>3</v>
       </c>
-      <c r="H107" s="85"/>
+      <c r="H107" s="74"/>
       <c r="I107" s="26">
         <v>3</v>
       </c>
-      <c r="J107" s="85"/>
+      <c r="J107" s="74"/>
       <c r="K107" s="31"/>
     </row>
     <row r="108" spans="1:11" ht="102.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -11630,14 +11630,14 @@
       <c r="G108" s="26">
         <v>3</v>
       </c>
-      <c r="H108" s="83">
+      <c r="H108" s="73">
         <f>AVERAGE(G108:G109)</f>
         <v>3</v>
       </c>
       <c r="I108" s="26">
         <v>3</v>
       </c>
-      <c r="J108" s="83">
+      <c r="J108" s="73">
         <f>AVERAGE(I108:I109)</f>
         <v>3</v>
       </c>
@@ -11657,11 +11657,11 @@
       <c r="G109" s="26">
         <v>3</v>
       </c>
-      <c r="H109" s="85"/>
+      <c r="H109" s="74"/>
       <c r="I109" s="26">
         <v>3</v>
       </c>
-      <c r="J109" s="85"/>
+      <c r="J109" s="74"/>
       <c r="K109" s="31"/>
     </row>
     <row r="110" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -11686,14 +11686,14 @@
       <c r="G110" s="26">
         <v>3</v>
       </c>
-      <c r="H110" s="83">
+      <c r="H110" s="73">
         <f>AVERAGE(G110:G111)</f>
         <v>3</v>
       </c>
       <c r="I110" s="26">
         <v>3</v>
       </c>
-      <c r="J110" s="83">
+      <c r="J110" s="73">
         <f>AVERAGE(I110:I111)</f>
         <v>3</v>
       </c>
@@ -11713,11 +11713,11 @@
       <c r="G111" s="26">
         <v>3</v>
       </c>
-      <c r="H111" s="85"/>
+      <c r="H111" s="74"/>
       <c r="I111" s="26">
         <v>3</v>
       </c>
-      <c r="J111" s="85"/>
+      <c r="J111" s="74"/>
       <c r="K111" s="31"/>
     </row>
     <row r="112" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11742,14 +11742,14 @@
       <c r="G112" s="26">
         <v>3</v>
       </c>
-      <c r="H112" s="83">
+      <c r="H112" s="73">
         <f>AVERAGE(G112:G113)</f>
         <v>3</v>
       </c>
       <c r="I112" s="26">
         <v>3</v>
       </c>
-      <c r="J112" s="83">
+      <c r="J112" s="73">
         <f>AVERAGE(I112:I113)</f>
         <v>3</v>
       </c>
@@ -11769,11 +11769,11 @@
       <c r="G113" s="26">
         <v>3</v>
       </c>
-      <c r="H113" s="85"/>
+      <c r="H113" s="74"/>
       <c r="I113" s="26">
         <v>3</v>
       </c>
-      <c r="J113" s="85"/>
+      <c r="J113" s="74"/>
       <c r="K113" s="31"/>
     </row>
     <row r="114" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11833,14 +11833,14 @@
       <c r="G115" s="26">
         <v>2</v>
       </c>
-      <c r="H115" s="83">
+      <c r="H115" s="73">
         <f>AVERAGE(G115:G122)</f>
         <v>2.5</v>
       </c>
       <c r="I115" s="26">
         <v>3</v>
       </c>
-      <c r="J115" s="83">
+      <c r="J115" s="73">
         <f>AVERAGE(I115:I122)</f>
         <v>3</v>
       </c>
@@ -11860,11 +11860,11 @@
       <c r="G116" s="26">
         <v>3</v>
       </c>
-      <c r="H116" s="84"/>
+      <c r="H116" s="75"/>
       <c r="I116" s="26">
         <v>3</v>
       </c>
-      <c r="J116" s="84"/>
+      <c r="J116" s="75"/>
       <c r="K116" s="31"/>
     </row>
     <row r="117" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11880,11 +11880,11 @@
       <c r="G117" s="26">
         <v>2</v>
       </c>
-      <c r="H117" s="84"/>
+      <c r="H117" s="75"/>
       <c r="I117" s="26">
         <v>3</v>
       </c>
-      <c r="J117" s="84"/>
+      <c r="J117" s="75"/>
       <c r="K117" s="31"/>
     </row>
     <row r="118" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -11900,11 +11900,11 @@
       <c r="G118" s="26">
         <v>3</v>
       </c>
-      <c r="H118" s="84"/>
+      <c r="H118" s="75"/>
       <c r="I118" s="26">
         <v>3</v>
       </c>
-      <c r="J118" s="84"/>
+      <c r="J118" s="75"/>
       <c r="K118" s="31"/>
     </row>
     <row r="119" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11920,11 +11920,11 @@
       <c r="G119" s="26">
         <v>2</v>
       </c>
-      <c r="H119" s="84"/>
+      <c r="H119" s="75"/>
       <c r="I119" s="26">
         <v>3</v>
       </c>
-      <c r="J119" s="84"/>
+      <c r="J119" s="75"/>
       <c r="K119" s="31"/>
     </row>
     <row r="120" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11940,11 +11940,11 @@
       <c r="G120" s="26">
         <v>3</v>
       </c>
-      <c r="H120" s="84"/>
+      <c r="H120" s="75"/>
       <c r="I120" s="26">
         <v>3</v>
       </c>
-      <c r="J120" s="84"/>
+      <c r="J120" s="75"/>
       <c r="K120" s="31"/>
     </row>
     <row r="121" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -11960,11 +11960,11 @@
       <c r="G121" s="26">
         <v>2</v>
       </c>
-      <c r="H121" s="84"/>
+      <c r="H121" s="75"/>
       <c r="I121" s="26">
         <v>3</v>
       </c>
-      <c r="J121" s="84"/>
+      <c r="J121" s="75"/>
       <c r="K121" s="31"/>
     </row>
     <row r="122" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -11980,11 +11980,11 @@
       <c r="G122" s="26">
         <v>3</v>
       </c>
-      <c r="H122" s="84"/>
+      <c r="H122" s="75"/>
       <c r="I122" s="26">
         <v>3</v>
       </c>
-      <c r="J122" s="84"/>
+      <c r="J122" s="75"/>
       <c r="K122" s="31"/>
     </row>
     <row r="123" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -12001,11 +12001,11 @@
       <c r="G123" s="26">
         <v>2</v>
       </c>
-      <c r="H123" s="85"/>
+      <c r="H123" s="74"/>
       <c r="I123" s="26">
         <v>3</v>
       </c>
-      <c r="J123" s="85"/>
+      <c r="J123" s="74"/>
       <c r="K123" s="31"/>
     </row>
     <row r="124" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.35">
@@ -12030,14 +12030,14 @@
       <c r="G124" s="23">
         <v>3</v>
       </c>
-      <c r="H124" s="83">
+      <c r="H124" s="73">
         <f>AVERAGE(G124:G126)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I124" s="23">
         <v>3</v>
       </c>
-      <c r="J124" s="83">
+      <c r="J124" s="73">
         <f>AVERAGE(I124:I126)</f>
         <v>3</v>
       </c>
@@ -12057,11 +12057,11 @@
       <c r="G125" s="24">
         <v>3</v>
       </c>
-      <c r="H125" s="84"/>
+      <c r="H125" s="75"/>
       <c r="I125" s="24">
         <v>3</v>
       </c>
-      <c r="J125" s="84"/>
+      <c r="J125" s="75"/>
       <c r="K125" s="31"/>
     </row>
     <row r="126" spans="1:11" ht="41.4" thickBot="1" x14ac:dyDescent="0.4">
@@ -12078,11 +12078,11 @@
       <c r="G126" s="25">
         <v>1</v>
       </c>
-      <c r="H126" s="85"/>
+      <c r="H126" s="74"/>
       <c r="I126" s="25">
         <v>3</v>
       </c>
-      <c r="J126" s="85"/>
+      <c r="J126" s="74"/>
       <c r="K126" s="31"/>
     </row>
     <row r="127" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -12107,14 +12107,14 @@
       <c r="G127" s="26">
         <v>3</v>
       </c>
-      <c r="H127" s="83">
+      <c r="H127" s="73">
         <f>AVERAGE(G127:G128)</f>
         <v>3</v>
       </c>
       <c r="I127" s="26">
         <v>3</v>
       </c>
-      <c r="J127" s="83">
+      <c r="J127" s="73">
         <f>AVERAGE(I127:I128)</f>
         <v>3</v>
       </c>
@@ -12134,11 +12134,11 @@
       <c r="G128" s="26">
         <v>3</v>
       </c>
-      <c r="H128" s="85"/>
+      <c r="H128" s="74"/>
       <c r="I128" s="26">
         <v>3</v>
       </c>
-      <c r="J128" s="85"/>
+      <c r="J128" s="74"/>
       <c r="K128" s="31"/>
     </row>
     <row r="129" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -12163,14 +12163,14 @@
       <c r="G129" s="23">
         <v>1</v>
       </c>
-      <c r="H129" s="83">
+      <c r="H129" s="73">
         <f>AVERAGE(G129:G133)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I129" s="23">
         <v>3</v>
       </c>
-      <c r="J129" s="83">
+      <c r="J129" s="73">
         <f>AVERAGE(I129:I133)</f>
         <v>3</v>
       </c>
@@ -12190,11 +12190,11 @@
       <c r="G130" s="24">
         <v>2</v>
       </c>
-      <c r="H130" s="84"/>
+      <c r="H130" s="75"/>
       <c r="I130" s="24">
         <v>3</v>
       </c>
-      <c r="J130" s="84"/>
+      <c r="J130" s="75"/>
       <c r="K130" s="31"/>
     </row>
     <row r="131" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -12210,11 +12210,11 @@
       <c r="G131" s="24">
         <v>2</v>
       </c>
-      <c r="H131" s="84"/>
+      <c r="H131" s="75"/>
       <c r="I131" s="24">
         <v>3</v>
       </c>
-      <c r="J131" s="84"/>
+      <c r="J131" s="75"/>
       <c r="K131" s="31"/>
     </row>
     <row r="132" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.35">
@@ -12230,11 +12230,11 @@
       <c r="G132" s="24">
         <v>3</v>
       </c>
-      <c r="H132" s="84"/>
+      <c r="H132" s="75"/>
       <c r="I132" s="24">
         <v>3</v>
       </c>
-      <c r="J132" s="84"/>
+      <c r="J132" s="75"/>
       <c r="K132" s="31"/>
     </row>
     <row r="133" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -12251,11 +12251,11 @@
       <c r="G133" s="25">
         <v>3</v>
       </c>
-      <c r="H133" s="85"/>
+      <c r="H133" s="74"/>
       <c r="I133" s="25">
         <v>3</v>
       </c>
-      <c r="J133" s="85"/>
+      <c r="J133" s="74"/>
       <c r="K133" s="31"/>
     </row>
     <row r="134" spans="1:11" ht="122.4" x14ac:dyDescent="0.35">
@@ -12280,14 +12280,14 @@
       <c r="G134" s="23">
         <v>3</v>
       </c>
-      <c r="H134" s="83">
+      <c r="H134" s="73">
         <f>AVERAGE(G134:G137)</f>
         <v>3</v>
       </c>
       <c r="I134" s="23">
         <v>3</v>
       </c>
-      <c r="J134" s="83">
+      <c r="J134" s="73">
         <f>AVERAGE(I134:I137)</f>
         <v>3</v>
       </c>
@@ -12307,11 +12307,11 @@
       <c r="G135" s="24">
         <v>3</v>
       </c>
-      <c r="H135" s="84"/>
+      <c r="H135" s="75"/>
       <c r="I135" s="24">
         <v>3</v>
       </c>
-      <c r="J135" s="84"/>
+      <c r="J135" s="75"/>
       <c r="K135" s="31"/>
     </row>
     <row r="136" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -12327,11 +12327,11 @@
       <c r="G136" s="24">
         <v>3</v>
       </c>
-      <c r="H136" s="84"/>
+      <c r="H136" s="75"/>
       <c r="I136" s="24">
         <v>3</v>
       </c>
-      <c r="J136" s="84"/>
+      <c r="J136" s="75"/>
       <c r="K136" s="31"/>
     </row>
     <row r="137" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -12348,11 +12348,11 @@
       <c r="G137" s="25">
         <v>3</v>
       </c>
-      <c r="H137" s="85"/>
+      <c r="H137" s="74"/>
       <c r="I137" s="25">
         <v>3</v>
       </c>
-      <c r="J137" s="85"/>
+      <c r="J137" s="74"/>
       <c r="K137" s="31"/>
     </row>
     <row r="138" spans="1:11" ht="332.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12447,14 +12447,14 @@
       <c r="G140" s="26">
         <v>3</v>
       </c>
-      <c r="H140" s="83">
+      <c r="H140" s="73">
         <f>AVERAGE(G140:G141)</f>
         <v>3</v>
       </c>
       <c r="I140" s="26">
         <v>3</v>
       </c>
-      <c r="J140" s="83">
+      <c r="J140" s="73">
         <f>AVERAGE(I140:I141)</f>
         <v>3</v>
       </c>
@@ -12474,11 +12474,11 @@
       <c r="G141" s="26">
         <v>3</v>
       </c>
-      <c r="H141" s="85"/>
+      <c r="H141" s="74"/>
       <c r="I141" s="26">
         <v>3</v>
       </c>
-      <c r="J141" s="85"/>
+      <c r="J141" s="74"/>
       <c r="K141" s="31"/>
     </row>
     <row r="142" spans="1:11" ht="82.2" thickBot="1" x14ac:dyDescent="0.4">
@@ -12503,14 +12503,14 @@
       <c r="G142" s="26">
         <v>3</v>
       </c>
-      <c r="H142" s="83">
+      <c r="H142" s="73">
         <f>AVERAGE(G142:G143)</f>
         <v>3</v>
       </c>
       <c r="I142" s="26">
         <v>3</v>
       </c>
-      <c r="J142" s="83">
+      <c r="J142" s="73">
         <f>AVERAGE(I142:I143)</f>
         <v>3</v>
       </c>
@@ -12530,11 +12530,11 @@
       <c r="G143" s="26">
         <v>3</v>
       </c>
-      <c r="H143" s="85"/>
+      <c r="H143" s="74"/>
       <c r="I143" s="26">
         <v>3</v>
       </c>
-      <c r="J143" s="85"/>
+      <c r="J143" s="74"/>
       <c r="K143" s="31"/>
     </row>
     <row r="144" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.35">
@@ -12559,14 +12559,14 @@
       <c r="G144" s="23">
         <v>3</v>
       </c>
-      <c r="H144" s="83">
+      <c r="H144" s="73">
         <f>AVERAGE(G144:G147)</f>
         <v>3</v>
       </c>
       <c r="I144" s="23">
         <v>3</v>
       </c>
-      <c r="J144" s="83">
+      <c r="J144" s="73">
         <f>AVERAGE(I144:I147)</f>
         <v>3</v>
       </c>
@@ -12586,11 +12586,11 @@
       <c r="G145" s="24">
         <v>3</v>
       </c>
-      <c r="H145" s="84"/>
+      <c r="H145" s="75"/>
       <c r="I145" s="24">
         <v>3</v>
       </c>
-      <c r="J145" s="84"/>
+      <c r="J145" s="75"/>
       <c r="K145" s="31"/>
     </row>
     <row r="146" spans="1:11" ht="22.2" x14ac:dyDescent="0.35">
@@ -12606,11 +12606,11 @@
       <c r="G146" s="24">
         <v>3</v>
       </c>
-      <c r="H146" s="84"/>
+      <c r="H146" s="75"/>
       <c r="I146" s="24">
         <v>3</v>
       </c>
-      <c r="J146" s="84"/>
+      <c r="J146" s="75"/>
       <c r="K146" s="31"/>
     </row>
     <row r="147" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12627,11 +12627,11 @@
       <c r="G147" s="25">
         <v>3</v>
       </c>
-      <c r="H147" s="85"/>
+      <c r="H147" s="74"/>
       <c r="I147" s="25">
         <v>3</v>
       </c>
-      <c r="J147" s="85"/>
+      <c r="J147" s="74"/>
       <c r="K147" s="31"/>
     </row>
     <row r="148" spans="1:11" ht="372" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12656,14 +12656,14 @@
       <c r="G148" s="26">
         <v>3</v>
       </c>
-      <c r="H148" s="83">
+      <c r="H148" s="73">
         <f>AVERAGE(G148:G149)</f>
         <v>3</v>
       </c>
       <c r="I148" s="26">
         <v>3</v>
       </c>
-      <c r="J148" s="83">
+      <c r="J148" s="73">
         <f>AVERAGE(I148:I149)</f>
         <v>3</v>
       </c>
@@ -12683,11 +12683,11 @@
       <c r="G149" s="26">
         <v>3</v>
       </c>
-      <c r="H149" s="85"/>
+      <c r="H149" s="74"/>
       <c r="I149" s="26">
         <v>3</v>
       </c>
-      <c r="J149" s="85"/>
+      <c r="J149" s="74"/>
       <c r="K149" s="31"/>
     </row>
     <row r="150" spans="1:11" ht="217.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -12712,14 +12712,14 @@
       <c r="G150" s="23">
         <v>1</v>
       </c>
-      <c r="H150" s="83">
+      <c r="H150" s="73">
         <f>AVERAGE(G150:G153)</f>
         <v>1.5</v>
       </c>
       <c r="I150" s="23">
         <v>3</v>
       </c>
-      <c r="J150" s="83">
+      <c r="J150" s="73">
         <f>AVERAGE(I150:I153)</f>
         <v>3</v>
       </c>
@@ -12739,11 +12739,11 @@
       <c r="G151" s="24">
         <v>2</v>
       </c>
-      <c r="H151" s="84"/>
+      <c r="H151" s="75"/>
       <c r="I151" s="24">
         <v>3</v>
       </c>
-      <c r="J151" s="84"/>
+      <c r="J151" s="75"/>
       <c r="K151" s="31"/>
     </row>
     <row r="152" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -12759,11 +12759,11 @@
       <c r="G152" s="24">
         <v>2</v>
       </c>
-      <c r="H152" s="84"/>
+      <c r="H152" s="75"/>
       <c r="I152" s="24">
         <v>3</v>
       </c>
-      <c r="J152" s="84"/>
+      <c r="J152" s="75"/>
       <c r="K152" s="31"/>
     </row>
     <row r="153" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -12780,11 +12780,11 @@
       <c r="G153" s="25">
         <v>1</v>
       </c>
-      <c r="H153" s="85"/>
+      <c r="H153" s="74"/>
       <c r="I153" s="25">
         <v>3</v>
       </c>
-      <c r="J153" s="85"/>
+      <c r="J153" s="74"/>
       <c r="K153" s="31"/>
     </row>
     <row r="154" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -12809,14 +12809,14 @@
       <c r="G154" s="23">
         <v>3</v>
       </c>
-      <c r="H154" s="83">
+      <c r="H154" s="73">
         <f>AVERAGE(G154:G155)</f>
         <v>3</v>
       </c>
       <c r="I154" s="23">
         <v>3</v>
       </c>
-      <c r="J154" s="83">
+      <c r="J154" s="73">
         <f>AVERAGE(I154:I155)</f>
         <v>3</v>
       </c>
@@ -12836,11 +12836,11 @@
       <c r="G155" s="25">
         <v>3</v>
       </c>
-      <c r="H155" s="85"/>
+      <c r="H155" s="74"/>
       <c r="I155" s="25">
         <v>3</v>
       </c>
-      <c r="J155" s="85"/>
+      <c r="J155" s="74"/>
       <c r="K155" s="31"/>
     </row>
     <row r="156" spans="1:11" ht="102" x14ac:dyDescent="0.35">
@@ -12865,14 +12865,14 @@
       <c r="G156" s="23">
         <v>3</v>
       </c>
-      <c r="H156" s="83">
+      <c r="H156" s="73">
         <f>AVERAGE(G156:G159)</f>
         <v>3</v>
       </c>
       <c r="I156" s="23">
         <v>3</v>
       </c>
-      <c r="J156" s="83">
+      <c r="J156" s="73">
         <f>AVERAGE(I156:I159)</f>
         <v>3</v>
       </c>
@@ -12892,11 +12892,11 @@
       <c r="G157" s="24">
         <v>3</v>
       </c>
-      <c r="H157" s="84"/>
+      <c r="H157" s="75"/>
       <c r="I157" s="24">
         <v>3</v>
       </c>
-      <c r="J157" s="84"/>
+      <c r="J157" s="75"/>
       <c r="K157" s="31"/>
     </row>
     <row r="158" spans="1:11" ht="22.2" x14ac:dyDescent="0.35">
@@ -12912,11 +12912,11 @@
       <c r="G158" s="24">
         <v>3</v>
       </c>
-      <c r="H158" s="84"/>
+      <c r="H158" s="75"/>
       <c r="I158" s="24">
         <v>3</v>
       </c>
-      <c r="J158" s="84"/>
+      <c r="J158" s="75"/>
       <c r="K158" s="31"/>
     </row>
     <row r="159" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -12933,11 +12933,11 @@
       <c r="G159" s="25">
         <v>3</v>
       </c>
-      <c r="H159" s="85"/>
+      <c r="H159" s="74"/>
       <c r="I159" s="25">
         <v>3</v>
       </c>
-      <c r="J159" s="85"/>
+      <c r="J159" s="74"/>
       <c r="K159" s="31"/>
     </row>
     <row r="160" spans="1:11" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12997,14 +12997,14 @@
       <c r="G161" s="23">
         <v>1</v>
       </c>
-      <c r="H161" s="83">
+      <c r="H161" s="73">
         <f>AVERAGE(G161:G165)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I161" s="23">
         <v>3</v>
       </c>
-      <c r="J161" s="83">
+      <c r="J161" s="73">
         <f>AVERAGE(I161:I165)</f>
         <v>3</v>
       </c>
@@ -13024,11 +13024,11 @@
       <c r="G162" s="24">
         <v>2</v>
       </c>
-      <c r="H162" s="84"/>
+      <c r="H162" s="75"/>
       <c r="I162" s="24">
         <v>3</v>
       </c>
-      <c r="J162" s="84"/>
+      <c r="J162" s="75"/>
       <c r="K162" s="31"/>
     </row>
     <row r="163" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -13044,11 +13044,11 @@
       <c r="G163" s="24">
         <v>2</v>
       </c>
-      <c r="H163" s="84"/>
+      <c r="H163" s="75"/>
       <c r="I163" s="24">
         <v>3</v>
       </c>
-      <c r="J163" s="84"/>
+      <c r="J163" s="75"/>
       <c r="K163" s="31"/>
     </row>
     <row r="164" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -13064,11 +13064,11 @@
       <c r="G164" s="24">
         <v>3</v>
       </c>
-      <c r="H164" s="84"/>
+      <c r="H164" s="75"/>
       <c r="I164" s="24">
         <v>3</v>
       </c>
-      <c r="J164" s="84"/>
+      <c r="J164" s="75"/>
       <c r="K164" s="31"/>
     </row>
     <row r="165" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13085,11 +13085,11 @@
       <c r="G165" s="25">
         <v>3</v>
       </c>
-      <c r="H165" s="85"/>
+      <c r="H165" s="74"/>
       <c r="I165" s="25">
         <v>3</v>
       </c>
-      <c r="J165" s="85"/>
+      <c r="J165" s="74"/>
       <c r="K165" s="31"/>
     </row>
     <row r="166" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.35">
@@ -13114,14 +13114,14 @@
       <c r="G166" s="23">
         <v>1</v>
       </c>
-      <c r="H166" s="83">
+      <c r="H166" s="73">
         <f>AVERAGE(G166:G170)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I166" s="23">
         <v>3</v>
       </c>
-      <c r="J166" s="83">
+      <c r="J166" s="73">
         <f>AVERAGE(I166:I170)</f>
         <v>3</v>
       </c>
@@ -13141,11 +13141,11 @@
       <c r="G167" s="24">
         <v>2</v>
       </c>
-      <c r="H167" s="84"/>
+      <c r="H167" s="75"/>
       <c r="I167" s="24">
         <v>3</v>
       </c>
-      <c r="J167" s="84"/>
+      <c r="J167" s="75"/>
       <c r="K167" s="31"/>
     </row>
     <row r="168" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -13161,11 +13161,11 @@
       <c r="G168" s="24">
         <v>2</v>
       </c>
-      <c r="H168" s="84"/>
+      <c r="H168" s="75"/>
       <c r="I168" s="24">
         <v>3</v>
       </c>
-      <c r="J168" s="84"/>
+      <c r="J168" s="75"/>
       <c r="K168" s="31"/>
     </row>
     <row r="169" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -13181,11 +13181,11 @@
       <c r="G169" s="24">
         <v>3</v>
       </c>
-      <c r="H169" s="84"/>
+      <c r="H169" s="75"/>
       <c r="I169" s="24">
         <v>3</v>
       </c>
-      <c r="J169" s="84"/>
+      <c r="J169" s="75"/>
       <c r="K169" s="31"/>
     </row>
     <row r="170" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13202,11 +13202,11 @@
       <c r="G170" s="25">
         <v>3</v>
       </c>
-      <c r="H170" s="85"/>
+      <c r="H170" s="74"/>
       <c r="I170" s="25">
         <v>3</v>
       </c>
-      <c r="J170" s="85"/>
+      <c r="J170" s="74"/>
       <c r="K170" s="31"/>
     </row>
     <row r="171" spans="1:11" ht="288" customHeight="1" x14ac:dyDescent="0.35">
@@ -13231,14 +13231,14 @@
       <c r="G171" s="23">
         <v>3</v>
       </c>
-      <c r="H171" s="83">
+      <c r="H171" s="73">
         <f>AVERAGE(G171:G174)</f>
         <v>3</v>
       </c>
       <c r="I171" s="23">
         <v>3</v>
       </c>
-      <c r="J171" s="83">
+      <c r="J171" s="73">
         <f>AVERAGE(I171:I174)</f>
         <v>3</v>
       </c>
@@ -13258,11 +13258,11 @@
       <c r="G172" s="24">
         <v>3</v>
       </c>
-      <c r="H172" s="84"/>
+      <c r="H172" s="75"/>
       <c r="I172" s="24">
         <v>3</v>
       </c>
-      <c r="J172" s="84"/>
+      <c r="J172" s="75"/>
       <c r="K172" s="31"/>
     </row>
     <row r="173" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -13278,11 +13278,11 @@
       <c r="G173" s="24">
         <v>3</v>
       </c>
-      <c r="H173" s="84"/>
+      <c r="H173" s="75"/>
       <c r="I173" s="24">
         <v>3</v>
       </c>
-      <c r="J173" s="84"/>
+      <c r="J173" s="75"/>
       <c r="K173" s="31"/>
     </row>
     <row r="174" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13299,11 +13299,11 @@
       <c r="G174" s="25">
         <v>3</v>
       </c>
-      <c r="H174" s="85"/>
+      <c r="H174" s="74"/>
       <c r="I174" s="25">
         <v>3</v>
       </c>
-      <c r="J174" s="85"/>
+      <c r="J174" s="74"/>
       <c r="K174" s="31"/>
     </row>
     <row r="175" spans="1:11" ht="81.599999999999994" x14ac:dyDescent="0.35">
@@ -13328,14 +13328,14 @@
       <c r="G175" s="23">
         <v>1</v>
       </c>
-      <c r="H175" s="83">
+      <c r="H175" s="73">
         <f>AVERAGE(G175:G179)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I175" s="23">
         <v>3</v>
       </c>
-      <c r="J175" s="83">
+      <c r="J175" s="73">
         <f>AVERAGE(I175:I179)</f>
         <v>3</v>
       </c>
@@ -13355,11 +13355,11 @@
       <c r="G176" s="24">
         <v>2</v>
       </c>
-      <c r="H176" s="84"/>
+      <c r="H176" s="75"/>
       <c r="I176" s="24">
         <v>3</v>
       </c>
-      <c r="J176" s="84"/>
+      <c r="J176" s="75"/>
       <c r="K176" s="31"/>
     </row>
     <row r="177" spans="1:11" ht="22.2" x14ac:dyDescent="0.35">
@@ -13375,11 +13375,11 @@
       <c r="G177" s="24">
         <v>2</v>
       </c>
-      <c r="H177" s="84"/>
+      <c r="H177" s="75"/>
       <c r="I177" s="24">
         <v>3</v>
       </c>
-      <c r="J177" s="84"/>
+      <c r="J177" s="75"/>
       <c r="K177" s="31"/>
     </row>
     <row r="178" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -13395,11 +13395,11 @@
       <c r="G178" s="24">
         <v>3</v>
       </c>
-      <c r="H178" s="84"/>
+      <c r="H178" s="75"/>
       <c r="I178" s="24">
         <v>3</v>
       </c>
-      <c r="J178" s="84"/>
+      <c r="J178" s="75"/>
       <c r="K178" s="31"/>
     </row>
     <row r="179" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13416,11 +13416,11 @@
       <c r="G179" s="25">
         <v>3</v>
       </c>
-      <c r="H179" s="85"/>
+      <c r="H179" s="74"/>
       <c r="I179" s="25">
         <v>3</v>
       </c>
-      <c r="J179" s="85"/>
+      <c r="J179" s="74"/>
       <c r="K179" s="31"/>
     </row>
     <row r="180" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13445,14 +13445,14 @@
       <c r="G180" s="26">
         <v>3</v>
       </c>
-      <c r="H180" s="83">
+      <c r="H180" s="73">
         <f>AVERAGE(G180:G181)</f>
         <v>3</v>
       </c>
       <c r="I180" s="26">
         <v>3</v>
       </c>
-      <c r="J180" s="83">
+      <c r="J180" s="73">
         <f>AVERAGE(I180:I181)</f>
         <v>3</v>
       </c>
@@ -13472,11 +13472,11 @@
       <c r="G181" s="26">
         <v>3</v>
       </c>
-      <c r="H181" s="85"/>
+      <c r="H181" s="74"/>
       <c r="I181" s="26">
         <v>3</v>
       </c>
-      <c r="J181" s="85"/>
+      <c r="J181" s="74"/>
       <c r="K181" s="31"/>
     </row>
     <row r="182" spans="1:11" ht="390" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13536,14 +13536,14 @@
       <c r="G183" s="26">
         <v>3</v>
       </c>
-      <c r="H183" s="83">
+      <c r="H183" s="73">
         <f>AVERAGE(G183:G184)</f>
         <v>3</v>
       </c>
       <c r="I183" s="26">
         <v>3</v>
       </c>
-      <c r="J183" s="83">
+      <c r="J183" s="73">
         <f>AVERAGE(I183:I184)</f>
         <v>3</v>
       </c>
@@ -13563,11 +13563,11 @@
       <c r="G184" s="26">
         <v>3</v>
       </c>
-      <c r="H184" s="85"/>
+      <c r="H184" s="74"/>
       <c r="I184" s="26">
         <v>3</v>
       </c>
-      <c r="J184" s="85"/>
+      <c r="J184" s="74"/>
       <c r="K184" s="31"/>
     </row>
     <row r="185" spans="1:11" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13592,14 +13592,14 @@
       <c r="G185" s="26">
         <v>3</v>
       </c>
-      <c r="H185" s="83">
+      <c r="H185" s="73">
         <f>AVERAGE(G185:G186)</f>
         <v>3</v>
       </c>
       <c r="I185" s="26">
         <v>3</v>
       </c>
-      <c r="J185" s="83">
+      <c r="J185" s="73">
         <f>AVERAGE(I185:I186)</f>
         <v>3</v>
       </c>
@@ -13619,11 +13619,11 @@
       <c r="G186" s="26">
         <v>3</v>
       </c>
-      <c r="H186" s="85"/>
+      <c r="H186" s="74"/>
       <c r="I186" s="26">
         <v>3</v>
       </c>
-      <c r="J186" s="85"/>
+      <c r="J186" s="74"/>
       <c r="K186" s="31"/>
     </row>
     <row r="187" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.35">
@@ -13648,14 +13648,14 @@
       <c r="G187" s="23">
         <v>3</v>
       </c>
-      <c r="H187" s="83">
+      <c r="H187" s="73">
         <f>AVERAGE(G187:G189)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I187" s="23">
         <v>3</v>
       </c>
-      <c r="J187" s="83">
+      <c r="J187" s="73">
         <f>AVERAGE(I187:I189)</f>
         <v>3</v>
       </c>
@@ -13675,11 +13675,11 @@
       <c r="G188" s="24">
         <v>3</v>
       </c>
-      <c r="H188" s="84"/>
+      <c r="H188" s="75"/>
       <c r="I188" s="24">
         <v>3</v>
       </c>
-      <c r="J188" s="84"/>
+      <c r="J188" s="75"/>
       <c r="K188" s="31"/>
     </row>
     <row r="189" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13696,11 +13696,11 @@
       <c r="G189" s="25">
         <v>1</v>
       </c>
-      <c r="H189" s="85"/>
+      <c r="H189" s="74"/>
       <c r="I189" s="25">
         <v>3</v>
       </c>
-      <c r="J189" s="85"/>
+      <c r="J189" s="74"/>
       <c r="K189" s="31"/>
     </row>
     <row r="190" spans="1:11" ht="61.2" x14ac:dyDescent="0.35">
@@ -13725,14 +13725,14 @@
       <c r="G190" s="23">
         <v>3</v>
       </c>
-      <c r="H190" s="83">
+      <c r="H190" s="73">
         <f>AVERAGE(G190:G192)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I190" s="23">
         <v>3</v>
       </c>
-      <c r="J190" s="83">
+      <c r="J190" s="73">
         <f>AVERAGE(I190:I192)</f>
         <v>3</v>
       </c>
@@ -13752,11 +13752,11 @@
       <c r="G191" s="24">
         <v>3</v>
       </c>
-      <c r="H191" s="84"/>
+      <c r="H191" s="75"/>
       <c r="I191" s="24">
         <v>3</v>
       </c>
-      <c r="J191" s="84"/>
+      <c r="J191" s="75"/>
       <c r="K191" s="31"/>
     </row>
     <row r="192" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13773,11 +13773,11 @@
       <c r="G192" s="25">
         <v>1</v>
       </c>
-      <c r="H192" s="85"/>
+      <c r="H192" s="74"/>
       <c r="I192" s="25">
         <v>3</v>
       </c>
-      <c r="J192" s="85"/>
+      <c r="J192" s="74"/>
       <c r="K192" s="31"/>
     </row>
     <row r="193" spans="1:11" ht="102" x14ac:dyDescent="0.35">
@@ -13802,14 +13802,14 @@
       <c r="G193" s="23">
         <v>3</v>
       </c>
-      <c r="H193" s="83">
+      <c r="H193" s="73">
         <f>AVERAGE(G193:G195)</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="I193" s="23">
         <v>3</v>
       </c>
-      <c r="J193" s="83">
+      <c r="J193" s="73">
         <f>AVERAGE(I193:I195)</f>
         <v>3</v>
       </c>
@@ -13829,11 +13829,11 @@
       <c r="G194" s="24">
         <v>3</v>
       </c>
-      <c r="H194" s="84"/>
+      <c r="H194" s="75"/>
       <c r="I194" s="24">
         <v>3</v>
       </c>
-      <c r="J194" s="84"/>
+      <c r="J194" s="75"/>
       <c r="K194" s="31"/>
     </row>
     <row r="195" spans="1:11" ht="22.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13850,11 +13850,11 @@
       <c r="G195" s="25">
         <v>1</v>
       </c>
-      <c r="H195" s="85"/>
+      <c r="H195" s="74"/>
       <c r="I195" s="25">
         <v>3</v>
       </c>
-      <c r="J195" s="85"/>
+      <c r="J195" s="74"/>
       <c r="K195" s="31"/>
     </row>
     <row r="196" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13879,14 +13879,14 @@
       <c r="G196" s="26">
         <v>3</v>
       </c>
-      <c r="H196" s="83">
+      <c r="H196" s="73">
         <f>AVERAGE(G196:G197)</f>
         <v>3</v>
       </c>
       <c r="I196" s="26">
         <v>3</v>
       </c>
-      <c r="J196" s="83">
+      <c r="J196" s="73">
         <f>AVERAGE(I196:I197)</f>
         <v>3</v>
       </c>
@@ -13906,11 +13906,11 @@
       <c r="G197" s="26">
         <v>3</v>
       </c>
-      <c r="H197" s="85"/>
+      <c r="H197" s="74"/>
       <c r="I197" s="26">
         <v>3</v>
       </c>
-      <c r="J197" s="85"/>
+      <c r="J197" s="74"/>
       <c r="K197" s="31"/>
     </row>
     <row r="198" spans="1:11" ht="61.8" thickBot="1" x14ac:dyDescent="0.4">
@@ -13935,14 +13935,14 @@
       <c r="G198" s="26">
         <v>3</v>
       </c>
-      <c r="H198" s="83">
+      <c r="H198" s="73">
         <f>AVERAGE(G198:G199)</f>
         <v>3</v>
       </c>
       <c r="I198" s="26">
         <v>3</v>
       </c>
-      <c r="J198" s="83">
+      <c r="J198" s="73">
         <f>AVERAGE(I198:I199)</f>
         <v>3</v>
       </c>
@@ -13962,68 +13962,49 @@
       <c r="G199" s="26">
         <v>3</v>
       </c>
-      <c r="H199" s="85"/>
+      <c r="H199" s="74"/>
       <c r="I199" s="26">
         <v>3</v>
       </c>
-      <c r="J199" s="85"/>
+      <c r="J199" s="74"/>
       <c r="K199" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="111">
-    <mergeCell ref="H187:H189"/>
-    <mergeCell ref="H190:H192"/>
-    <mergeCell ref="H193:H195"/>
-    <mergeCell ref="H196:H197"/>
-    <mergeCell ref="H198:H199"/>
-    <mergeCell ref="H171:H174"/>
-    <mergeCell ref="H175:H179"/>
-    <mergeCell ref="H180:H181"/>
-    <mergeCell ref="H183:H184"/>
-    <mergeCell ref="H185:H186"/>
-    <mergeCell ref="H150:H153"/>
-    <mergeCell ref="H154:H155"/>
-    <mergeCell ref="H156:H159"/>
-    <mergeCell ref="H161:H165"/>
-    <mergeCell ref="H166:H170"/>
-    <mergeCell ref="H134:H137"/>
-    <mergeCell ref="H140:H141"/>
-    <mergeCell ref="H142:H143"/>
-    <mergeCell ref="H144:H147"/>
-    <mergeCell ref="H148:H149"/>
-    <mergeCell ref="H112:H113"/>
-    <mergeCell ref="H115:H123"/>
-    <mergeCell ref="H124:H126"/>
-    <mergeCell ref="H127:H128"/>
-    <mergeCell ref="H129:H133"/>
-    <mergeCell ref="H88:H90"/>
-    <mergeCell ref="H91:H105"/>
-    <mergeCell ref="H106:H107"/>
-    <mergeCell ref="H108:H109"/>
-    <mergeCell ref="H110:H111"/>
-    <mergeCell ref="H75:H77"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="H83:H84"/>
-    <mergeCell ref="H86:H87"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="H56:H58"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="H64:H68"/>
-    <mergeCell ref="H72:H73"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="H49:H53"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="J44:J46"/>
-    <mergeCell ref="J56:J58"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="J41:J43"/>
+    <mergeCell ref="J31:J32"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="J14:J18"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J196:J197"/>
+    <mergeCell ref="J198:J199"/>
+    <mergeCell ref="J148:J149"/>
+    <mergeCell ref="J180:J181"/>
+    <mergeCell ref="J183:J184"/>
+    <mergeCell ref="J150:J153"/>
+    <mergeCell ref="J156:J159"/>
+    <mergeCell ref="J171:J174"/>
+    <mergeCell ref="J161:J165"/>
+    <mergeCell ref="J166:J170"/>
+    <mergeCell ref="J190:J192"/>
+    <mergeCell ref="J193:J195"/>
+    <mergeCell ref="J187:J189"/>
+    <mergeCell ref="J154:J155"/>
+    <mergeCell ref="J175:J179"/>
     <mergeCell ref="J91:J105"/>
     <mergeCell ref="J144:J147"/>
     <mergeCell ref="J134:J137"/>
@@ -14048,40 +14029,59 @@
     <mergeCell ref="J140:J141"/>
     <mergeCell ref="J115:J123"/>
     <mergeCell ref="J75:J77"/>
-    <mergeCell ref="J196:J197"/>
-    <mergeCell ref="J198:J199"/>
-    <mergeCell ref="J148:J149"/>
-    <mergeCell ref="J180:J181"/>
-    <mergeCell ref="J183:J184"/>
-    <mergeCell ref="J150:J153"/>
-    <mergeCell ref="J156:J159"/>
-    <mergeCell ref="J171:J174"/>
-    <mergeCell ref="J161:J165"/>
-    <mergeCell ref="J166:J170"/>
-    <mergeCell ref="J190:J192"/>
-    <mergeCell ref="J193:J195"/>
-    <mergeCell ref="J187:J189"/>
-    <mergeCell ref="J154:J155"/>
-    <mergeCell ref="J175:J179"/>
-    <mergeCell ref="J31:J32"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="J14:J18"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="J19:J22"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="H49:H53"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="J44:J46"/>
+    <mergeCell ref="J56:J58"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="J41:J43"/>
+    <mergeCell ref="H75:H77"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="H83:H84"/>
+    <mergeCell ref="H86:H87"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="H56:H58"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="H64:H68"/>
+    <mergeCell ref="H72:H73"/>
+    <mergeCell ref="H112:H113"/>
+    <mergeCell ref="H115:H123"/>
+    <mergeCell ref="H124:H126"/>
+    <mergeCell ref="H127:H128"/>
+    <mergeCell ref="H129:H133"/>
+    <mergeCell ref="H88:H90"/>
+    <mergeCell ref="H91:H105"/>
+    <mergeCell ref="H106:H107"/>
+    <mergeCell ref="H108:H109"/>
+    <mergeCell ref="H110:H111"/>
+    <mergeCell ref="H150:H153"/>
+    <mergeCell ref="H154:H155"/>
+    <mergeCell ref="H156:H159"/>
+    <mergeCell ref="H161:H165"/>
+    <mergeCell ref="H166:H170"/>
+    <mergeCell ref="H134:H137"/>
+    <mergeCell ref="H140:H141"/>
+    <mergeCell ref="H142:H143"/>
+    <mergeCell ref="H144:H147"/>
+    <mergeCell ref="H148:H149"/>
+    <mergeCell ref="H187:H189"/>
+    <mergeCell ref="H190:H192"/>
+    <mergeCell ref="H193:H195"/>
+    <mergeCell ref="H196:H197"/>
+    <mergeCell ref="H198:H199"/>
+    <mergeCell ref="H171:H174"/>
+    <mergeCell ref="H175:H179"/>
+    <mergeCell ref="H180:H181"/>
+    <mergeCell ref="H183:H184"/>
+    <mergeCell ref="H185:H186"/>
   </mergeCells>
   <conditionalFormatting sqref="J7">
     <cfRule type="cellIs" dxfId="437" priority="914" operator="between">
@@ -16142,9 +16142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15140C3A-C9BE-4ADC-A224-5E346724E143}">
   <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16215,7 +16213,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="204" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="244.8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -16315,7 +16313,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="122.4" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>2</v>
       </c>
@@ -16535,7 +16533,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="285.60000000000002" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>8</v>
       </c>
@@ -16715,7 +16713,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="224.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>13</v>
       </c>
@@ -16755,7 +16753,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="244.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>15</v>
       </c>
@@ -17235,7 +17233,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>30</v>
       </c>
@@ -17275,7 +17273,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="163.19999999999999" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>31</v>
       </c>
@@ -17535,7 +17533,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>39</v>
       </c>
@@ -17555,7 +17553,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>40</v>
       </c>
@@ -17615,7 +17613,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>41</v>
       </c>
@@ -17635,7 +17633,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>41</v>
       </c>
@@ -17695,7 +17693,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="122.4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.35">
       <c r="A78" s="8">
         <v>42</v>
       </c>
@@ -17735,7 +17733,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>43</v>
       </c>
@@ -17855,7 +17853,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>45</v>
       </c>
@@ -17875,7 +17873,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="61.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>45</v>
       </c>
@@ -17935,7 +17933,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>46</v>
       </c>
@@ -17955,7 +17953,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>47</v>
       </c>
@@ -18055,7 +18053,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>51</v>
       </c>
@@ -18095,7 +18093,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>51</v>
       </c>
@@ -18195,7 +18193,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>54</v>
       </c>
@@ -18275,7 +18273,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>57</v>
       </c>
@@ -18335,7 +18333,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>58</v>
       </c>
@@ -18415,7 +18413,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="326.39999999999998" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="367.2" x14ac:dyDescent="0.25">
       <c r="A114" s="8">
         <v>60</v>
       </c>
@@ -18495,7 +18493,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="163.19999999999999" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="183.6" x14ac:dyDescent="0.25">
       <c r="A118" s="8">
         <v>63</v>
       </c>
@@ -18555,7 +18553,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="102" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="122.4" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <v>64</v>
       </c>
@@ -18895,7 +18893,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="61.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.25">
       <c r="A138" s="8">
         <v>66</v>
       </c>
@@ -19135,7 +19133,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="244.8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
       <c r="A150" s="8">
         <v>71</v>
       </c>
@@ -19155,7 +19153,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="102" x14ac:dyDescent="0.25">
       <c r="A151" s="8">
         <v>71</v>
       </c>
@@ -19235,7 +19233,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="102" x14ac:dyDescent="0.25">
       <c r="A155" s="8">
         <v>71</v>
       </c>
@@ -19315,7 +19313,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="244.8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
       <c r="A159" s="8">
         <v>73</v>
       </c>
@@ -19335,7 +19333,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="224.4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
       <c r="A160" s="8">
         <v>73</v>
       </c>
@@ -19415,7 +19413,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="244.8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
       <c r="A164" s="8">
         <v>74</v>
       </c>
@@ -19535,7 +19533,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="265.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="285.60000000000002" x14ac:dyDescent="0.25">
       <c r="A170" s="8">
         <v>76</v>
       </c>
@@ -19615,7 +19613,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" ht="102" x14ac:dyDescent="0.35">
       <c r="A174" s="8">
         <v>79</v>
       </c>
@@ -19655,7 +19653,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="102" x14ac:dyDescent="0.25">
       <c r="A176" s="8">
         <v>80</v>
       </c>
@@ -20015,7 +20013,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="163.19999999999999" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="183.6" x14ac:dyDescent="0.25">
       <c r="A194" s="8">
         <v>86</v>
       </c>
@@ -20095,7 +20093,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="142.80000000000001" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="163.19999999999999" x14ac:dyDescent="0.25">
       <c r="A198" s="8">
         <v>87</v>
       </c>
@@ -20115,7 +20113,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="163.19999999999999" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="183.6" x14ac:dyDescent="0.25">
       <c r="A199" s="8">
         <v>87</v>
       </c>
@@ -20135,7 +20133,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="204" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A200" s="8">
         <v>87</v>
       </c>
@@ -20155,7 +20153,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="204" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A201" s="8">
         <v>87</v>
       </c>
@@ -20355,7 +20353,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="204" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A211" s="8">
         <v>89</v>
       </c>
@@ -20395,7 +20393,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="163.19999999999999" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="183.6" x14ac:dyDescent="0.25">
       <c r="A213" s="8">
         <v>90</v>
       </c>
@@ -20515,7 +20513,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" ht="102" x14ac:dyDescent="0.25">
       <c r="A219" s="8">
         <v>94</v>
       </c>
@@ -20575,7 +20573,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="61.2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A222" s="8">
         <v>95</v>
       </c>
@@ -20615,7 +20613,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="61.2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:6" ht="81.599999999999994" x14ac:dyDescent="0.35">
       <c r="A224" s="8">
         <v>95</v>
       </c>

</xml_diff>